<commit_message>
now reads in excel file with patient data and writes risk scores to another workbook
</commit_message>
<xml_diff>
--- a/lung-cancer-validator/three_model_excel_template.xlsx
+++ b/lung-cancer-validator/three_model_excel_template.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackallan/Dropbox/UROP/Knowledge Grid/LungCancerDataAPI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/natalielampa/Desktop/KGRID/KGridGitRepo/knowledge-objects/lung-cancer-validator/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1140" windowWidth="17760" windowHeight="17980" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="17760" windowHeight="15540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Patient Risk Scores" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -96,7 +97,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -108,6 +109,13 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -133,7 +141,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -142,6 +150,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U1"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -495,7 +506,149 @@
         <v>19</v>
       </c>
     </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4">
+        <v>50</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4">
+        <v>30</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0</v>
+      </c>
+      <c r="G2" s="4">
+        <v>0</v>
+      </c>
+      <c r="H2" s="4">
+        <v>0</v>
+      </c>
+      <c r="I2" s="4">
+        <v>50</v>
+      </c>
+      <c r="J2" s="4">
+        <v>1</v>
+      </c>
+      <c r="K2" s="4">
+        <v>30</v>
+      </c>
+      <c r="L2" s="4">
+        <v>1</v>
+      </c>
+      <c r="M2" s="4">
+        <v>0</v>
+      </c>
+      <c r="N2" s="4">
+        <v>0</v>
+      </c>
+      <c r="O2" s="4">
+        <v>0</v>
+      </c>
+      <c r="P2" s="4">
+        <v>50</v>
+      </c>
+      <c r="Q2" s="4">
+        <v>2</v>
+      </c>
+      <c r="R2" s="4">
+        <v>2</v>
+      </c>
+      <c r="S2" s="4">
+        <v>0</v>
+      </c>
+      <c r="T2" s="4">
+        <v>0</v>
+      </c>
+      <c r="U2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4">
+        <v>65</v>
+      </c>
+      <c r="C3" s="4">
+        <v>20</v>
+      </c>
+      <c r="D3" s="4">
+        <v>50</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0</v>
+      </c>
+      <c r="H3" s="4">
+        <v>0</v>
+      </c>
+      <c r="I3" s="4">
+        <v>65</v>
+      </c>
+      <c r="J3" s="4">
+        <v>1</v>
+      </c>
+      <c r="K3" s="4">
+        <v>50</v>
+      </c>
+      <c r="L3" s="4">
+        <v>20</v>
+      </c>
+      <c r="M3" s="4">
+        <v>0</v>
+      </c>
+      <c r="N3" s="4">
+        <v>0</v>
+      </c>
+      <c r="O3" s="4">
+        <v>0</v>
+      </c>
+      <c r="P3" s="4">
+        <v>65</v>
+      </c>
+      <c r="Q3" s="4">
+        <v>3</v>
+      </c>
+      <c r="R3" s="4">
+        <v>3</v>
+      </c>
+      <c r="S3" s="4">
+        <v>1</v>
+      </c>
+      <c r="T3" s="4">
+        <v>1</v>
+      </c>
+      <c r="U3" s="4">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>